<commit_message>
Update seed data resources and enhance status documentation
- Modified seed-data-resources.csv to standardize employee grade formatting from 'LEVEL_X' to 'LEVEL X'.
- Updated seed-data-resources.xlsx to reflect changes in the CSV file.
- Enhanced the status document to provide a comprehensive overview of pending requirements, including critical, high, medium, and non-functional tasks, along with their estimated efforts and completion statuses.
- Improved clarity in the documentation to facilitate better tracking of project progress and next steps.
</commit_message>
<xml_diff>
--- a/seed-data-resources.xlsx
+++ b/seed-data-resources.xlsx
@@ -511,7 +511,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>LEVEL_5</t>
+          <t>LEVEL 5</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -552,7 +552,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>LEVEL_6</t>
+          <t>LEVEL 6</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -597,7 +597,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>LEVEL_7</t>
+          <t>LEVEL 7</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -642,7 +642,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>LEVEL_5</t>
+          <t>LEVEL 5</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -687,7 +687,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>LEVEL_8</t>
+          <t>LEVEL 8</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -728,7 +728,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>LEVEL_6</t>
+          <t>LEVEL 6</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -773,7 +773,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>LEVEL_7</t>
+          <t>LEVEL 7</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -818,7 +818,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>LEVEL_5</t>
+          <t>LEVEL 5</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -863,7 +863,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>LEVEL_6</t>
+          <t>LEVEL 6</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -904,7 +904,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>LEVEL_7</t>
+          <t>LEVEL 7</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -949,7 +949,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>LEVEL_8</t>
+          <t>LEVEL 8</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -994,7 +994,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>LEVEL_5</t>
+          <t>LEVEL 5</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -1035,7 +1035,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>LEVEL_6</t>
+          <t>LEVEL 6</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -1080,7 +1080,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>LEVEL_7</t>
+          <t>LEVEL 7</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1121,7 +1121,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>LEVEL_5</t>
+          <t>LEVEL 5</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1166,7 +1166,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>LEVEL_8</t>
+          <t>LEVEL 8</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1211,7 +1211,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>LEVEL_6</t>
+          <t>LEVEL 6</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1256,7 +1256,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>LEVEL_7</t>
+          <t>LEVEL 7</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1297,7 +1297,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>LEVEL_5</t>
+          <t>LEVEL 5</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1338,7 +1338,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>LEVEL_6</t>
+          <t>LEVEL 6</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1383,7 +1383,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>LEVEL_7</t>
+          <t>LEVEL 7</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -1428,7 +1428,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>LEVEL_8</t>
+          <t>LEVEL 8</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -1473,7 +1473,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>LEVEL_5</t>
+          <t>LEVEL 5</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -1514,7 +1514,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>LEVEL_6</t>
+          <t>LEVEL 6</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -1555,7 +1555,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>LEVEL_7</t>
+          <t>LEVEL 7</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -1600,7 +1600,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>LEVEL_5</t>
+          <t>LEVEL 5</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -1645,7 +1645,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>LEVEL_8</t>
+          <t>LEVEL 8</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -1690,7 +1690,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>LEVEL_6</t>
+          <t>LEVEL 6</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -1731,7 +1731,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>LEVEL_7</t>
+          <t>LEVEL 7</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -1772,7 +1772,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>LEVEL_5</t>
+          <t>LEVEL 5</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">

</xml_diff>